<commit_message>
ReadMe, Data Dictionary and Pickle file listing participants and their groups.
</commit_message>
<xml_diff>
--- a/ReadMe and Data Dictionary.xlsx
+++ b/ReadMe and Data Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\GitHub\Day-Ahead-Electricity-Market-Modelling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3374002B-FEF0-48E4-83BE-3BD448732C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF29943A-A584-430F-B97D-353343F8A477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="960" windowWidth="29040" windowHeight="15720" xr2:uid="{C1341366-7860-43E0-A9AB-2E1E1259EFE0}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="333">
   <si>
     <t>DeliveryPeriod</t>
   </si>
@@ -671,12 +671,469 @@
     <t>modelling approaches we only utilise a subset of the explanatory variables).</t>
   </si>
   <si>
+    <t>As noted in the research paper, we exclude/ignore such trading periods.</t>
+  </si>
+  <si>
+    <t>- One zipped file relates to Approach 1, n = 4 data (i.e. dim = 2 * 2 * 4 = 16).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When a variable is listed in this tab, it does not mean it is necessarily used in the generation of a forecast (as discussed in the paper for some </t>
+  </si>
+  <si>
+    <t>Metered generation for the participant in trading period [DeliveryPeriod - 168 hours]</t>
+  </si>
+  <si>
+    <t>The IDA1 quantity bought or sold by the participant in trading period [DeliveryPeriod - 168 hours]</t>
+  </si>
+  <si>
+    <t>The IDA2 quantity bought or sold by the participant in trading period [DeliveryPeriod - 168 hours]</t>
+  </si>
+  <si>
+    <t>The IDA3 quantity bought or sold by the participant in trading period [DeliveryPeriod - 168 hours]</t>
+  </si>
+  <si>
+    <t>- Taking a zipped file, and decompressing it, will result in &gt; 400 csvs.</t>
+  </si>
+  <si>
+    <t>Each csv is specific to a participant in the Irish Day-Ahead electricity market.</t>
+  </si>
+  <si>
+    <t>Part of participants complex commercial order data (if relevant) for DeliveryPeriod, can be ignored.</t>
+  </si>
+  <si>
+    <t>Part of participants complex commercial order data (if relevant) for [DeliveryPeriod - 48 hours], can be ignored.</t>
+  </si>
+  <si>
+    <t>Part of participants complex commercial order data (if relevant) for [DeliveryPeriod - 72 hours], can be ignored.</t>
+  </si>
+  <si>
+    <t>Part of participants complex commercial order data (if relevant) for [DeliveryPeriod - 168 hours], can be ignored.</t>
+  </si>
+  <si>
+    <t>Participant's transformed target data for DeliveryPeriod</t>
+  </si>
+  <si>
+    <t>Participant's lagged transformed target  data (i.e. explanatory data)</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Lower</t>
+  </si>
+  <si>
+    <t>Quantile_0</t>
+  </si>
+  <si>
+    <t>Quantile_5</t>
+  </si>
+  <si>
+    <t>Quantile_10</t>
+  </si>
+  <si>
+    <t>Quantile_15</t>
+  </si>
+  <si>
+    <t>Quantile_20</t>
+  </si>
+  <si>
+    <t>Quantile_25</t>
+  </si>
+  <si>
+    <t>Quantile_30</t>
+  </si>
+  <si>
+    <t>Quantile_35</t>
+  </si>
+  <si>
+    <t>Quantile_40</t>
+  </si>
+  <si>
+    <t>Quantile_45</t>
+  </si>
+  <si>
+    <t>Quantile_50</t>
+  </si>
+  <si>
+    <t>Quantile_55</t>
+  </si>
+  <si>
+    <t>Quantile_60</t>
+  </si>
+  <si>
+    <t>Quantile_65</t>
+  </si>
+  <si>
+    <t>Quantile_70</t>
+  </si>
+  <si>
+    <t>Quantile_75</t>
+  </si>
+  <si>
+    <t>Quantile_80</t>
+  </si>
+  <si>
+    <t>Quantile_85</t>
+  </si>
+  <si>
+    <t>Quantile_90</t>
+  </si>
+  <si>
+    <t>Quantile_95</t>
+  </si>
+  <si>
+    <t>Quantile_100</t>
+  </si>
+  <si>
+    <t>Upper</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Minimum_-48</t>
+  </si>
+  <si>
+    <t>Lower_-48</t>
+  </si>
+  <si>
+    <t>Quantile_0_-48</t>
+  </si>
+  <si>
+    <t>Quantile_5_-48</t>
+  </si>
+  <si>
+    <t>Quantile_10_-48</t>
+  </si>
+  <si>
+    <t>Quantile_15_-48</t>
+  </si>
+  <si>
+    <t>Quantile_20_-48</t>
+  </si>
+  <si>
+    <t>Quantile_25_-48</t>
+  </si>
+  <si>
+    <t>Quantile_30_-48</t>
+  </si>
+  <si>
+    <t>Quantile_35_-48</t>
+  </si>
+  <si>
+    <t>Quantile_40_-48</t>
+  </si>
+  <si>
+    <t>Quantile_45_-48</t>
+  </si>
+  <si>
+    <t>Quantile_50_-48</t>
+  </si>
+  <si>
+    <t>Quantile_55_-48</t>
+  </si>
+  <si>
+    <t>Quantile_60_-48</t>
+  </si>
+  <si>
+    <t>Quantile_65_-48</t>
+  </si>
+  <si>
+    <t>Quantile_70_-48</t>
+  </si>
+  <si>
+    <t>Quantile_75_-48</t>
+  </si>
+  <si>
+    <t>Quantile_80_-48</t>
+  </si>
+  <si>
+    <t>Quantile_85_-48</t>
+  </si>
+  <si>
+    <t>Quantile_90_-48</t>
+  </si>
+  <si>
+    <t>Quantile_95_-48</t>
+  </si>
+  <si>
+    <t>Quantile_100_-48</t>
+  </si>
+  <si>
+    <t>Upper_-48</t>
+  </si>
+  <si>
+    <t>Maximum_-48</t>
+  </si>
+  <si>
+    <t>Minimum_-72</t>
+  </si>
+  <si>
+    <t>Lower_-72</t>
+  </si>
+  <si>
+    <t>Quantile_0_-72</t>
+  </si>
+  <si>
+    <t>Quantile_5_-72</t>
+  </si>
+  <si>
+    <t>Quantile_10_-72</t>
+  </si>
+  <si>
+    <t>Quantile_15_-72</t>
+  </si>
+  <si>
+    <t>Quantile_20_-72</t>
+  </si>
+  <si>
+    <t>Quantile_25_-72</t>
+  </si>
+  <si>
+    <t>Quantile_30_-72</t>
+  </si>
+  <si>
+    <t>Quantile_35_-72</t>
+  </si>
+  <si>
+    <t>Quantile_40_-72</t>
+  </si>
+  <si>
+    <t>Quantile_45_-72</t>
+  </si>
+  <si>
+    <t>Quantile_50_-72</t>
+  </si>
+  <si>
+    <t>Quantile_55_-72</t>
+  </si>
+  <si>
+    <t>Quantile_60_-72</t>
+  </si>
+  <si>
+    <t>Quantile_65_-72</t>
+  </si>
+  <si>
+    <t>Quantile_70_-72</t>
+  </si>
+  <si>
+    <t>Quantile_75_-72</t>
+  </si>
+  <si>
+    <t>Quantile_80_-72</t>
+  </si>
+  <si>
+    <t>Quantile_85_-72</t>
+  </si>
+  <si>
+    <t>Quantile_90_-72</t>
+  </si>
+  <si>
+    <t>Quantile_95_-72</t>
+  </si>
+  <si>
+    <t>Quantile_100_-72</t>
+  </si>
+  <si>
+    <t>Upper_-72</t>
+  </si>
+  <si>
+    <t>Maximum_-72</t>
+  </si>
+  <si>
+    <t>Minimum_-168</t>
+  </si>
+  <si>
+    <t>Lower_-168</t>
+  </si>
+  <si>
+    <t>Quantile_0_-168</t>
+  </si>
+  <si>
+    <t>Quantile_5_-168</t>
+  </si>
+  <si>
+    <t>Quantile_10_-168</t>
+  </si>
+  <si>
+    <t>Quantile_15_-168</t>
+  </si>
+  <si>
+    <t>Quantile_20_-168</t>
+  </si>
+  <si>
+    <t>Quantile_25_-168</t>
+  </si>
+  <si>
+    <t>Quantile_30_-168</t>
+  </si>
+  <si>
+    <t>Quantile_35_-168</t>
+  </si>
+  <si>
+    <t>Quantile_40_-168</t>
+  </si>
+  <si>
+    <t>Quantile_45_-168</t>
+  </si>
+  <si>
+    <t>Quantile_50_-168</t>
+  </si>
+  <si>
+    <t>Quantile_55_-168</t>
+  </si>
+  <si>
+    <t>Quantile_60_-168</t>
+  </si>
+  <si>
+    <t>Quantile_65_-168</t>
+  </si>
+  <si>
+    <t>Quantile_70_-168</t>
+  </si>
+  <si>
+    <t>Quantile_75_-168</t>
+  </si>
+  <si>
+    <t>Quantile_80_-168</t>
+  </si>
+  <si>
+    <t>Quantile_85_-168</t>
+  </si>
+  <si>
+    <t>Quantile_90_-168</t>
+  </si>
+  <si>
+    <t>Quantile_95_-168</t>
+  </si>
+  <si>
+    <t>Quantile_100_-168</t>
+  </si>
+  <si>
+    <t>Upper_-168</t>
+  </si>
+  <si>
+    <t>Maximum_-168</t>
+  </si>
+  <si>
+    <t>….......</t>
+  </si>
+  <si>
+    <t>Participants quantity at Quantile_0 * 0.5 price point in DeliveryPeriod, this is part of the target data.</t>
+  </si>
+  <si>
+    <t>Participants quantity at minimum price point in DeliveryPeriod, this is part of the target data.</t>
+  </si>
+  <si>
+    <t>Participants quantity at Quantile_0 price point in DeliveryPeriod, this is part of the target data.</t>
+  </si>
+  <si>
+    <t>Participants quantity at Quantile_100 price point in DeliveryPeriod, this is part of the target data.</t>
+  </si>
+  <si>
+    <t>Participants quantity at Quantile_100 * 1.5 price point in DeliveryPeriod, this is part of the target data.</t>
+  </si>
+  <si>
+    <t>Participants quantity at maximum price point in DeliveryPeriod, this is part of the target data.</t>
+  </si>
+  <si>
+    <t>Particiapnts target data, but lagged i.e. explanatory data.</t>
+  </si>
+  <si>
+    <t>Each row corresponds to a trading period (or what we call a DeliveryPeriod). The columns represent either explanatory or target variables which are described below (and in subsequent tabs).</t>
+  </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
     <r>
       <t>- "</t>
     </r>
     <r>
       <rPr>
-        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Explanatory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" tab: this tab provides a data dictionary for the majority of the explanatory variables. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>- "</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Approach 1 (n=4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" tab:  target and additional explanatory variables that are specific to Approach 1 with a choice of n =4.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>- "</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Approach 2 (dim = 25)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" tab: target and additional explanatory variables that are specific to Approach 2, the transformed order data was generated using market price data from trading periods [j-1, j, j+1] over the previous 20 days.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>- "</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Aptos Narrow"/>
@@ -697,14 +1154,8 @@
     </r>
   </si>
   <si>
-    <t>As noted in the research paper, we exclude/ignore such trading periods.</t>
-  </si>
-  <si>
-    <t>- One zipped file relates to Approach 1, n = 4 data (i.e. dim = 2 * 2 * 4 = 16).</t>
-  </si>
-  <si>
     <r>
-      <t>- "</t>
+      <t xml:space="preserve">-The </t>
     </r>
     <r>
       <rPr>
@@ -715,7 +1166,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Explanatory</t>
+      <t>"groups_and_participants.pickle</t>
     </r>
     <r>
       <rPr>
@@ -725,91 +1176,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">" tab: this tab provides a data dictionary for the majority of the explanatory variables. </t>
+      <t>" file lists the participants according to the various groups.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">When a variable is listed in this tab, it does not mean it is necessarily used in the generation of a forecast (as discussed in the paper for some </t>
-  </si>
-  <si>
-    <r>
-      <t>- "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Approach 1 (n=4)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" tab:  target and explanatory variables that are specific to Approach 1 with a choice of n =4.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>- "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Approach 2 (dim = 25)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" tab: target and explanatory variables that are specific to Approach 2, the transformed order data was generated using price quantile data from trading periods [j-1, j, j+1] over the previous 20 days.</t>
-    </r>
-  </si>
-  <si>
-    <t>Metered generation for the participant in trading period [DeliveryPeriod - 168 hours]</t>
-  </si>
-  <si>
-    <t>The IDA1 quantity bought or sold by the participant in trading period [DeliveryPeriod - 168 hours]</t>
-  </si>
-  <si>
-    <t>The IDA2 quantity bought or sold by the participant in trading period [DeliveryPeriod - 168 hours]</t>
-  </si>
-  <si>
-    <t>The IDA3 quantity bought or sold by the participant in trading period [DeliveryPeriod - 168 hours]</t>
-  </si>
-  <si>
-    <t>- Taking a zipped file, and decompressing it, will result in &gt; 400 csvs.</t>
-  </si>
-  <si>
-    <t>Each csv is specific to a participant in the Irish Day-Ahead electricity market.</t>
-  </si>
-  <si>
-    <t>Each row corresponds to a trading period (or what we call a delivery period). The columns represent either explanatory or target variables which are described below.</t>
+    <t>A complete description of the modelling approach, the data, the different groupsings (and how we assign participants to a group) is provided in the paper.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -842,6 +1220,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -863,7 +1250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -874,6 +1261,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1208,9 +1597,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49592C9E-DA42-4318-A0FA-2129C2EF1ED4}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1219,71 +1610,86 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>214</v>
+      <c r="A6" s="4" t="s">
+        <v>209</v>
       </c>
       <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>205</v>
+      <c r="A8" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>206</v>
+      <c r="A9" s="4" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>208</v>
+        <v>328</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>202</v>
+        <v>329</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>203</v>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -1295,8 +1701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8958FF4C-1CCA-43C5-B030-B3678480CD26}">
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63:B67"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1814,7 +2220,7 @@
         <v>130</v>
       </c>
       <c r="B64" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -1822,7 +2228,7 @@
         <v>131</v>
       </c>
       <c r="B65" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -1830,7 +2236,7 @@
         <v>132</v>
       </c>
       <c r="B66" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
@@ -1838,7 +2244,7 @@
         <v>133</v>
       </c>
       <c r="B67" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -1848,373 +2254,600 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3950C708-FD42-425A-AB4A-5FCC92BFFF2F}">
-  <dimension ref="A2:A73"/>
+  <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>128</v>
+      </c>
+      <c r="B73" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -2224,14 +2857,889 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA49D4D-6828-45B1-9BDA-5CAAA23BAC3C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="89" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>219</v>
+      </c>
+      <c r="B6" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>220</v>
+      </c>
+      <c r="B7" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B8" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B9" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>223</v>
+      </c>
+      <c r="B10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>224</v>
+      </c>
+      <c r="B11" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B12" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>226</v>
+      </c>
+      <c r="B13" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>227</v>
+      </c>
+      <c r="B14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>228</v>
+      </c>
+      <c r="B15" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>229</v>
+      </c>
+      <c r="B16" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>230</v>
+      </c>
+      <c r="B17" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>231</v>
+      </c>
+      <c r="B18" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>232</v>
+      </c>
+      <c r="B19" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>233</v>
+      </c>
+      <c r="B20" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>234</v>
+      </c>
+      <c r="B21" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>235</v>
+      </c>
+      <c r="B22" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>236</v>
+      </c>
+      <c r="B23" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>237</v>
+      </c>
+      <c r="B24" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>238</v>
+      </c>
+      <c r="B25" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>239</v>
+      </c>
+      <c r="B26" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>240</v>
+      </c>
+      <c r="B27" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>241</v>
+      </c>
+      <c r="B28" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>242</v>
+      </c>
+      <c r="B31" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>243</v>
+      </c>
+      <c r="B32" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>244</v>
+      </c>
+      <c r="B33" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>245</v>
+      </c>
+      <c r="B34" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>246</v>
+      </c>
+      <c r="B35" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>247</v>
+      </c>
+      <c r="B36" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>248</v>
+      </c>
+      <c r="B37" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>249</v>
+      </c>
+      <c r="B38" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>250</v>
+      </c>
+      <c r="B39" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>251</v>
+      </c>
+      <c r="B40" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>252</v>
+      </c>
+      <c r="B41" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>253</v>
+      </c>
+      <c r="B42" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>254</v>
+      </c>
+      <c r="B43" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>255</v>
+      </c>
+      <c r="B44" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>256</v>
+      </c>
+      <c r="B45" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>257</v>
+      </c>
+      <c r="B46" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>258</v>
+      </c>
+      <c r="B47" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>259</v>
+      </c>
+      <c r="B48" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>260</v>
+      </c>
+      <c r="B49" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>261</v>
+      </c>
+      <c r="B50" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>262</v>
+      </c>
+      <c r="B51" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>263</v>
+      </c>
+      <c r="B52" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>264</v>
+      </c>
+      <c r="B53" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>265</v>
+      </c>
+      <c r="B54" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>266</v>
+      </c>
+      <c r="B55" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>88</v>
+      </c>
+      <c r="B56" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>267</v>
+      </c>
+      <c r="B58" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>268</v>
+      </c>
+      <c r="B59" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>269</v>
+      </c>
+      <c r="B60" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>270</v>
+      </c>
+      <c r="B61" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>271</v>
+      </c>
+      <c r="B62" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>272</v>
+      </c>
+      <c r="B63" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>273</v>
+      </c>
+      <c r="B64" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>274</v>
+      </c>
+      <c r="B65" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>275</v>
+      </c>
+      <c r="B66" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>276</v>
+      </c>
+      <c r="B67" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>277</v>
+      </c>
+      <c r="B68" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>278</v>
+      </c>
+      <c r="B69" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>279</v>
+      </c>
+      <c r="B70" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>280</v>
+      </c>
+      <c r="B71" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>281</v>
+      </c>
+      <c r="B72" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>282</v>
+      </c>
+      <c r="B73" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>283</v>
+      </c>
+      <c r="B74" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>284</v>
+      </c>
+      <c r="B75" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>285</v>
+      </c>
+      <c r="B76" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>286</v>
+      </c>
+      <c r="B77" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>287</v>
+      </c>
+      <c r="B78" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>288</v>
+      </c>
+      <c r="B79" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>289</v>
+      </c>
+      <c r="B80" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>290</v>
+      </c>
+      <c r="B81" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>291</v>
+      </c>
+      <c r="B82" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>111</v>
+      </c>
+      <c r="B83" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>112</v>
+      </c>
+      <c r="B84" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>292</v>
+      </c>
+      <c r="B85" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>293</v>
+      </c>
+      <c r="B86" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>294</v>
+      </c>
+      <c r="B87" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>295</v>
+      </c>
+      <c r="B88" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>296</v>
+      </c>
+      <c r="B89" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>297</v>
+      </c>
+      <c r="B90" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>298</v>
+      </c>
+      <c r="B91" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>299</v>
+      </c>
+      <c r="B92" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>300</v>
+      </c>
+      <c r="B93" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>301</v>
+      </c>
+      <c r="B94" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>302</v>
+      </c>
+      <c r="B95" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>303</v>
+      </c>
+      <c r="B96" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>304</v>
+      </c>
+      <c r="B97" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>305</v>
+      </c>
+      <c r="B98" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>306</v>
+      </c>
+      <c r="B99" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>307</v>
+      </c>
+      <c r="B100" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>308</v>
+      </c>
+      <c r="B101" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>309</v>
+      </c>
+      <c r="B102" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>310</v>
+      </c>
+      <c r="B103" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>311</v>
+      </c>
+      <c r="B104" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>312</v>
+      </c>
+      <c r="B105" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>313</v>
+      </c>
+      <c r="B106" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>314</v>
+      </c>
+      <c r="B107" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>315</v>
+      </c>
+      <c r="B108" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>316</v>
+      </c>
+      <c r="B109" t="s">
+        <v>324</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>